<commit_message>
Changed Sample DB Data
</commit_message>
<xml_diff>
--- a/docs/Sample DB Data.xlsx
+++ b/docs/Sample DB Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\TIP\ITE 001\FINAL PROJ\EnrollMe\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EF38D1-C06C-41DD-9194-73CC78DA3BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF188CD-52DC-43FD-BD23-1EA0342BE3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{456103EC-7965-48E1-865D-F284B988141A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{456103EC-7965-48E1-865D-F284B988141A}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_enrollees" sheetId="1" r:id="rId1"/>
@@ -626,8 +626,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="00000000\-00000"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="00000000\-00000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -723,21 +723,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyAlignment="1">
@@ -747,14 +744,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -763,6 +757,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -828,9 +825,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <i val="0"/>
-      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -853,12 +853,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -956,13 +953,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1006,6 +1003,122 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="00000000\-00000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1024,122 +1137,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="00000000\-00000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1154,45 +1151,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{188CCF96-84A8-4B4B-95A3-38B0DB5BEAFF}" name="Table2" displayName="Table2" ref="A2:AK7" totalsRowShown="0" headerRowDxfId="48" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{188CCF96-84A8-4B4B-95A3-38B0DB5BEAFF}" name="Table2" displayName="Table2" ref="A2:AK7" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <tableColumns count="37">
-    <tableColumn id="1" xr3:uid="{D9CD30EE-C7F0-45F7-9E82-634670440220}" name="id" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{E7648FC1-61AC-4EC9-A771-17061CC5CDB3}" name="student_number" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{2D7A6B19-EB94-41E0-A4C5-3F5C086E18C9}" name="enrll_transactionId" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{56307ED9-F29B-4144-8D31-5C4FF6208433}" name="enrll_type" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{A4A03904-EAA2-4385-8688-49951C5D5597}" name="enrll_level" dataDxfId="82"/>
-    <tableColumn id="6" xr3:uid="{89958D10-9D1C-4C32-9256-59E06A3BE32F}" name="enrll_program" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{ACA20B3D-ABDA-429D-91C7-D1486091832C}" name="enrll_schoolYear" dataDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{4C6348B9-A174-4E18-A2D2-63751C3EA63D}" name="enrll_semester" dataDxfId="79"/>
-    <tableColumn id="9" xr3:uid="{2A3D0A34-A835-475D-9AC1-B29EA8CC4595}" name="enrll_firstName" dataDxfId="78"/>
-    <tableColumn id="10" xr3:uid="{ABA01853-D99C-44A6-8732-AA5A0C4F0965}" name="enrll_midName" dataDxfId="77"/>
-    <tableColumn id="11" xr3:uid="{FA516390-427A-4EE5-9F03-2B182FEDDD03}" name="enrll_lastName" dataDxfId="76"/>
-    <tableColumn id="12" xr3:uid="{CD8E2B67-5568-4D17-9A20-162EE781A334}" name="enrll_suffixName" dataDxfId="75"/>
-    <tableColumn id="13" xr3:uid="{B9A82B88-2E4A-479B-A65F-D95E561127B1}" name="enrll_sex" dataDxfId="74"/>
-    <tableColumn id="14" xr3:uid="{604694F8-E920-41B1-B51F-735B8FD79C2F}" name="enrll_DoB" dataDxfId="73"/>
-    <tableColumn id="15" xr3:uid="{2E3BE1A1-1617-400A-A71D-C5B1EF191D13}" name="enrll_PoB" dataDxfId="72"/>
-    <tableColumn id="16" xr3:uid="{9A19B62C-8066-4887-8EA7-6A020CF379A8}" name="enrll_religion" dataDxfId="71"/>
-    <tableColumn id="17" xr3:uid="{D78B38FB-D2C4-491C-8B1A-828502E9312D}" name="enrll_nationality" dataDxfId="70"/>
-    <tableColumn id="18" xr3:uid="{B0DEBDD3-DD1C-4FB9-8EE5-62B4B9C28E2D}" name="enrll_civilStatus" dataDxfId="69"/>
-    <tableColumn id="19" xr3:uid="{A8A7CE98-2C2B-4BD6-A732-03C3CE557DA2}" name="enrll_country" dataDxfId="68"/>
-    <tableColumn id="20" xr3:uid="{7C549A3E-9F96-4497-AB52-A843B2099C9E}" name="enrll_province" dataDxfId="67"/>
-    <tableColumn id="21" xr3:uid="{0F58FD1B-E0D1-4F12-BF24-10CFDC0E8AFD}" name="enrll_cityMun" dataDxfId="66"/>
-    <tableColumn id="22" xr3:uid="{33B4EA61-4AD6-465F-BB83-9A5C4B42363E}" name="enrll_brgy" dataDxfId="65"/>
-    <tableColumn id="23" xr3:uid="{AF3F6948-0BE6-458C-A08F-983A392BD409}" name="enrll_zipCode" dataDxfId="64"/>
-    <tableColumn id="24" xr3:uid="{2D894819-153B-4CEA-9774-31309BA351F8}" name="enrll_addrLine" dataDxfId="63"/>
-    <tableColumn id="25" xr3:uid="{3D580FD8-7F4D-47F6-BBC3-041C0BAC7E7E}" name="enrll_mobileNumber" dataDxfId="62"/>
-    <tableColumn id="26" xr3:uid="{8AB5599C-E968-4DF8-A6F5-50AA998E5F2B}" name="enrll_telephoneNumber" dataDxfId="61"/>
-    <tableColumn id="27" xr3:uid="{37B9282F-E729-44A5-9E46-76E3270D3B86}" name="enrll_email" dataDxfId="60" dataCellStyle="Hyperlink"/>
-    <tableColumn id="28" xr3:uid="{4A657144-098F-4634-98BE-6E42DB33F4FD}" name="grdn_firstName" dataDxfId="59"/>
-    <tableColumn id="29" xr3:uid="{6280AAA7-481A-494C-A56C-99ECB7E9F624}" name="grdn_midName" dataDxfId="58"/>
-    <tableColumn id="30" xr3:uid="{185EA602-31B1-4F68-9490-9E1B4D42403A}" name="grdn_lastName" dataDxfId="57"/>
-    <tableColumn id="31" xr3:uid="{354E8183-D732-4FE7-B312-A60A1247D00B}" name="grdn_suffixName" dataDxfId="56"/>
-    <tableColumn id="32" xr3:uid="{0AE34112-046D-4EFE-AAAA-5C7BBFAECACB}" name="grdn_sex" dataDxfId="55"/>
-    <tableColumn id="33" xr3:uid="{23F7BB9C-337D-4ABA-9C57-F679352858BF}" name="grdn_relation" dataDxfId="54"/>
-    <tableColumn id="34" xr3:uid="{68DB536B-529B-4036-9EC9-78FF85658DC5}" name="grn_address" dataDxfId="53"/>
-    <tableColumn id="35" xr3:uid="{BAE344A7-AA13-4C03-8238-4559945A2C36}" name="grn_mobileNumber" dataDxfId="52"/>
-    <tableColumn id="36" xr3:uid="{60CA15E2-1452-484F-A657-689B331D7BBA}" name="grn_telephoneNumber" dataDxfId="51"/>
-    <tableColumn id="37" xr3:uid="{D5DCCF22-C33B-4A8E-AD39-8C91C9FAEAB7}" name="grn_email" dataDxfId="50" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{D9CD30EE-C7F0-45F7-9E82-634670440220}" name="id" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{E7648FC1-61AC-4EC9-A771-17061CC5CDB3}" name="student_number" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{2D7A6B19-EB94-41E0-A4C5-3F5C086E18C9}" name="enrll_transactionId" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{56307ED9-F29B-4144-8D31-5C4FF6208433}" name="enrll_type" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{A4A03904-EAA2-4385-8688-49951C5D5597}" name="enrll_level" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{89958D10-9D1C-4C32-9256-59E06A3BE32F}" name="enrll_program" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{ACA20B3D-ABDA-429D-91C7-D1486091832C}" name="enrll_schoolYear" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{4C6348B9-A174-4E18-A2D2-63751C3EA63D}" name="enrll_semester" dataDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{2A3D0A34-A835-475D-9AC1-B29EA8CC4595}" name="enrll_firstName" dataDxfId="76"/>
+    <tableColumn id="10" xr3:uid="{ABA01853-D99C-44A6-8732-AA5A0C4F0965}" name="enrll_midName" dataDxfId="75"/>
+    <tableColumn id="11" xr3:uid="{FA516390-427A-4EE5-9F03-2B182FEDDD03}" name="enrll_lastName" dataDxfId="74"/>
+    <tableColumn id="12" xr3:uid="{CD8E2B67-5568-4D17-9A20-162EE781A334}" name="enrll_suffixName" dataDxfId="73"/>
+    <tableColumn id="13" xr3:uid="{B9A82B88-2E4A-479B-A65F-D95E561127B1}" name="enrll_sex" dataDxfId="72"/>
+    <tableColumn id="14" xr3:uid="{604694F8-E920-41B1-B51F-735B8FD79C2F}" name="enrll_DoB" dataDxfId="71"/>
+    <tableColumn id="15" xr3:uid="{2E3BE1A1-1617-400A-A71D-C5B1EF191D13}" name="enrll_PoB" dataDxfId="70"/>
+    <tableColumn id="16" xr3:uid="{9A19B62C-8066-4887-8EA7-6A020CF379A8}" name="enrll_religion" dataDxfId="69"/>
+    <tableColumn id="17" xr3:uid="{D78B38FB-D2C4-491C-8B1A-828502E9312D}" name="enrll_nationality" dataDxfId="68"/>
+    <tableColumn id="18" xr3:uid="{B0DEBDD3-DD1C-4FB9-8EE5-62B4B9C28E2D}" name="enrll_civilStatus" dataDxfId="67"/>
+    <tableColumn id="19" xr3:uid="{A8A7CE98-2C2B-4BD6-A732-03C3CE557DA2}" name="enrll_country" dataDxfId="66"/>
+    <tableColumn id="20" xr3:uid="{7C549A3E-9F96-4497-AB52-A843B2099C9E}" name="enrll_province" dataDxfId="65"/>
+    <tableColumn id="21" xr3:uid="{0F58FD1B-E0D1-4F12-BF24-10CFDC0E8AFD}" name="enrll_cityMun" dataDxfId="64"/>
+    <tableColumn id="22" xr3:uid="{33B4EA61-4AD6-465F-BB83-9A5C4B42363E}" name="enrll_brgy" dataDxfId="63"/>
+    <tableColumn id="23" xr3:uid="{AF3F6948-0BE6-458C-A08F-983A392BD409}" name="enrll_zipCode" dataDxfId="62"/>
+    <tableColumn id="24" xr3:uid="{2D894819-153B-4CEA-9774-31309BA351F8}" name="enrll_addrLine" dataDxfId="61"/>
+    <tableColumn id="25" xr3:uid="{3D580FD8-7F4D-47F6-BBC3-041C0BAC7E7E}" name="enrll_mobileNumber" dataDxfId="60"/>
+    <tableColumn id="26" xr3:uid="{8AB5599C-E968-4DF8-A6F5-50AA998E5F2B}" name="enrll_telephoneNumber" dataDxfId="59"/>
+    <tableColumn id="27" xr3:uid="{37B9282F-E729-44A5-9E46-76E3270D3B86}" name="enrll_email" dataDxfId="58" dataCellStyle="Hyperlink"/>
+    <tableColumn id="28" xr3:uid="{4A657144-098F-4634-98BE-6E42DB33F4FD}" name="grdn_firstName" dataDxfId="57"/>
+    <tableColumn id="29" xr3:uid="{6280AAA7-481A-494C-A56C-99ECB7E9F624}" name="grdn_midName" dataDxfId="56"/>
+    <tableColumn id="30" xr3:uid="{185EA602-31B1-4F68-9490-9E1B4D42403A}" name="grdn_lastName" dataDxfId="55"/>
+    <tableColumn id="31" xr3:uid="{354E8183-D732-4FE7-B312-A60A1247D00B}" name="grdn_suffixName" dataDxfId="54"/>
+    <tableColumn id="32" xr3:uid="{0AE34112-046D-4EFE-AAAA-5C7BBFAECACB}" name="grdn_sex" dataDxfId="53"/>
+    <tableColumn id="33" xr3:uid="{23F7BB9C-337D-4ABA-9C57-F679352858BF}" name="grdn_relation" dataDxfId="52"/>
+    <tableColumn id="34" xr3:uid="{68DB536B-529B-4036-9EC9-78FF85658DC5}" name="grn_address" dataDxfId="51"/>
+    <tableColumn id="35" xr3:uid="{BAE344A7-AA13-4C03-8238-4559945A2C36}" name="grn_mobileNumber" dataDxfId="50"/>
+    <tableColumn id="36" xr3:uid="{60CA15E2-1452-484F-A657-689B331D7BBA}" name="grn_telephoneNumber" dataDxfId="49"/>
+    <tableColumn id="37" xr3:uid="{D5DCCF22-C33B-4A8E-AD39-8C91C9FAEAB7}" name="grn_email" dataDxfId="48" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1202,37 +1199,37 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{02DA6F91-13A2-49C4-BD38-650AFFC75FFB}" name="Table24" displayName="Table24" ref="A2:AF5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <tableColumns count="32">
     <tableColumn id="2" xr3:uid="{4CDE91C0-D8EC-4AC3-ADF7-C903FD9396C7}" name="student_number" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{66F0BA32-1510-40D2-9C29-E64097F030FF}" name="enrll_level" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{8AEDD57F-D4A6-43D9-B412-CB1749108BF6}" name="enrll_program" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{9816A2CC-BF55-4D95-8FC9-C4B4DF8ED2ED}" name="enrll_firstName" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{219ACDD5-E75E-4960-9D59-83DAE164518D}" name="enrll_midName" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{0E742245-DE32-4E8E-AFF4-567D72A52DB0}" name="enrll_lastName" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{B5A373BF-BA8D-4C5E-A5DA-5B54B09A668F}" name="enrll_suffixName" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{48716A68-DDD0-4748-B351-24B7E264F89A}" name="enrll_sex" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{BDD4DE89-088E-44A3-AEA5-551EA82921C4}" name="enrll_DoB" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{03F9CAE6-DB03-4995-A44E-870CDDE011C5}" name="enrll_PoB" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{03ED354F-63A8-4573-966D-C5D4C4A8CE7C}" name="enrll_religion" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{1A251583-01C4-4BDE-BA83-2A82E85CC52D}" name="enrll_nationality" dataDxfId="36"/>
-    <tableColumn id="18" xr3:uid="{37465ACE-CFC0-499C-8532-B0B0A47CBD31}" name="enrll_civilStatus" dataDxfId="35"/>
-    <tableColumn id="19" xr3:uid="{0161A379-6256-41CB-9619-4874F73879AE}" name="enrll_country" dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{BC3DE766-862E-4573-A63F-044E061988CD}" name="enrll_province" dataDxfId="33"/>
-    <tableColumn id="21" xr3:uid="{8C68E05B-559E-439F-824A-CCDA2F4EB6C0}" name="enrll_cityMun" dataDxfId="32"/>
-    <tableColumn id="22" xr3:uid="{4374A8CE-1BA5-4C44-83C3-F384DAFE1DB3}" name="enrll_brgy" dataDxfId="31"/>
-    <tableColumn id="23" xr3:uid="{0E6D2E5F-5B19-40AA-B870-0E93DD517ACA}" name="enrll_zipCode" dataDxfId="30"/>
-    <tableColumn id="24" xr3:uid="{53884A20-EEE4-475E-8609-17C7206DA747}" name="enrll_addrLine" dataDxfId="29"/>
-    <tableColumn id="25" xr3:uid="{C98C7DAB-9F8F-4AA4-96B4-834A7FA12DB4}" name="enrll_mobileNumber" dataDxfId="28"/>
-    <tableColumn id="26" xr3:uid="{C4D66636-8F15-4E78-9EEF-7F61DC6F9322}" name="enrll_telephoneNumber" dataDxfId="27"/>
-    <tableColumn id="27" xr3:uid="{47AAE36D-9F1A-45D4-AFE6-E21D28699240}" name="enrll_email" dataDxfId="26" dataCellStyle="Hyperlink"/>
-    <tableColumn id="28" xr3:uid="{DE8C66BC-38F5-448E-8172-FDACBABEA02E}" name="grdn_firstName" dataDxfId="25"/>
-    <tableColumn id="29" xr3:uid="{62E0DE06-D351-467C-B859-BA7854964C5A}" name="grdn_midName" dataDxfId="24"/>
-    <tableColumn id="30" xr3:uid="{A81F08A9-B58D-48A3-A1F9-409E97BF638D}" name="grdn_lastName" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{B95CB64A-3112-4944-BD10-0D134A15240D}" name="grdn_suffixName" dataDxfId="22"/>
-    <tableColumn id="32" xr3:uid="{01F01CC7-D7D2-4AE5-A30D-DBF405013DEF}" name="grdn_sex" dataDxfId="21"/>
-    <tableColumn id="33" xr3:uid="{1A8C1BD1-DBC0-4DEB-B741-E8195560B6E9}" name="grdn_relation" dataDxfId="20"/>
-    <tableColumn id="34" xr3:uid="{E4037304-8DA5-445C-B0AA-203B60D18794}" name="grn_address" dataDxfId="19"/>
-    <tableColumn id="35" xr3:uid="{4791EC50-506E-41F6-8F75-D37F3B2A50CD}" name="grn_mobileNumber" dataDxfId="18"/>
-    <tableColumn id="36" xr3:uid="{1C44D570-FAB3-4138-BC02-B22503D67C28}" name="grn_telephoneNumber" dataDxfId="17"/>
-    <tableColumn id="37" xr3:uid="{578A081A-75C7-4DA1-B334-5FCE1F1DF16F}" name="grn_email" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{66F0BA32-1510-40D2-9C29-E64097F030FF}" name="enrll_level" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{8AEDD57F-D4A6-43D9-B412-CB1749108BF6}" name="enrll_program" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{9816A2CC-BF55-4D95-8FC9-C4B4DF8ED2ED}" name="enrll_firstName" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{219ACDD5-E75E-4960-9D59-83DAE164518D}" name="enrll_midName" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{0E742245-DE32-4E8E-AFF4-567D72A52DB0}" name="enrll_lastName" dataDxfId="40"/>
+    <tableColumn id="12" xr3:uid="{B5A373BF-BA8D-4C5E-A5DA-5B54B09A668F}" name="enrll_suffixName" dataDxfId="39"/>
+    <tableColumn id="13" xr3:uid="{48716A68-DDD0-4748-B351-24B7E264F89A}" name="enrll_sex" dataDxfId="38"/>
+    <tableColumn id="14" xr3:uid="{BDD4DE89-088E-44A3-AEA5-551EA82921C4}" name="enrll_DoB" dataDxfId="37"/>
+    <tableColumn id="15" xr3:uid="{03F9CAE6-DB03-4995-A44E-870CDDE011C5}" name="enrll_PoB" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{03ED354F-63A8-4573-966D-C5D4C4A8CE7C}" name="enrll_religion" dataDxfId="35"/>
+    <tableColumn id="17" xr3:uid="{1A251583-01C4-4BDE-BA83-2A82E85CC52D}" name="enrll_nationality" dataDxfId="34"/>
+    <tableColumn id="18" xr3:uid="{37465ACE-CFC0-499C-8532-B0B0A47CBD31}" name="enrll_civilStatus" dataDxfId="33"/>
+    <tableColumn id="19" xr3:uid="{0161A379-6256-41CB-9619-4874F73879AE}" name="enrll_country" dataDxfId="32"/>
+    <tableColumn id="20" xr3:uid="{BC3DE766-862E-4573-A63F-044E061988CD}" name="enrll_province" dataDxfId="31"/>
+    <tableColumn id="21" xr3:uid="{8C68E05B-559E-439F-824A-CCDA2F4EB6C0}" name="enrll_cityMun" dataDxfId="30"/>
+    <tableColumn id="22" xr3:uid="{4374A8CE-1BA5-4C44-83C3-F384DAFE1DB3}" name="enrll_brgy" dataDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{0E6D2E5F-5B19-40AA-B870-0E93DD517ACA}" name="enrll_zipCode" dataDxfId="28"/>
+    <tableColumn id="24" xr3:uid="{53884A20-EEE4-475E-8609-17C7206DA747}" name="enrll_addrLine" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{C98C7DAB-9F8F-4AA4-96B4-834A7FA12DB4}" name="enrll_mobileNumber" dataDxfId="26"/>
+    <tableColumn id="26" xr3:uid="{C4D66636-8F15-4E78-9EEF-7F61DC6F9322}" name="enrll_telephoneNumber" dataDxfId="25"/>
+    <tableColumn id="27" xr3:uid="{47AAE36D-9F1A-45D4-AFE6-E21D28699240}" name="enrll_email" dataDxfId="24" dataCellStyle="Hyperlink"/>
+    <tableColumn id="28" xr3:uid="{DE8C66BC-38F5-448E-8172-FDACBABEA02E}" name="grdn_firstName" dataDxfId="23"/>
+    <tableColumn id="29" xr3:uid="{62E0DE06-D351-467C-B859-BA7854964C5A}" name="grdn_midName" dataDxfId="22"/>
+    <tableColumn id="30" xr3:uid="{A81F08A9-B58D-48A3-A1F9-409E97BF638D}" name="grdn_lastName" dataDxfId="21"/>
+    <tableColumn id="31" xr3:uid="{B95CB64A-3112-4944-BD10-0D134A15240D}" name="grdn_suffixName" dataDxfId="20"/>
+    <tableColumn id="32" xr3:uid="{01F01CC7-D7D2-4AE5-A30D-DBF405013DEF}" name="grdn_sex" dataDxfId="19"/>
+    <tableColumn id="33" xr3:uid="{1A8C1BD1-DBC0-4DEB-B741-E8195560B6E9}" name="grdn_relation" dataDxfId="18"/>
+    <tableColumn id="34" xr3:uid="{E4037304-8DA5-445C-B0AA-203B60D18794}" name="grn_address" dataDxfId="17"/>
+    <tableColumn id="35" xr3:uid="{4791EC50-506E-41F6-8F75-D37F3B2A50CD}" name="grn_mobileNumber" dataDxfId="16"/>
+    <tableColumn id="36" xr3:uid="{1C44D570-FAB3-4138-BC02-B22503D67C28}" name="grn_telephoneNumber" dataDxfId="15"/>
+    <tableColumn id="37" xr3:uid="{578A081A-75C7-4DA1-B334-5FCE1F1DF16F}" name="grn_email" dataDxfId="14" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1241,12 +1238,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABC9AAFD-4A2F-4CEF-AE61-6785D6A9A483}" name="Table245" displayName="Table245" ref="A2:F31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="6">
-    <tableColumn id="5" xr3:uid="{7BBBCBD3-78C1-4F0C-856B-3E830B05560C}" name="course_code" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{24EF4C1F-BEE8-4E41-930E-4FFFDB057F32}" name="course_title" dataDxfId="6"/>
-    <tableColumn id="39" xr3:uid="{31821E7D-41CE-4FD9-9738-BC8C2DAD98C7}" name="lecture_units" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{F71578E7-7264-47F3-8533-E38F4E3086D5}" name="lab_units" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{DB43FBC9-574E-46D4-9BFB-9B523088C17E}" name="prerequisite" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{6DDA1655-AEBF-413D-A7EA-16517298FC61}" name="corequisite" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{7BBBCBD3-78C1-4F0C-856B-3E830B05560C}" name="course_code" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{24EF4C1F-BEE8-4E41-930E-4FFFDB057F32}" name="course_title" dataDxfId="10"/>
+    <tableColumn id="39" xr3:uid="{31821E7D-41CE-4FD9-9738-BC8C2DAD98C7}" name="lecture_units" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{F71578E7-7264-47F3-8533-E38F4E3086D5}" name="lab_units" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{DB43FBC9-574E-46D4-9BFB-9B523088C17E}" name="prerequisite" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{6DDA1655-AEBF-413D-A7EA-16517298FC61}" name="corequisite" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1563,15 +1560,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91B594-80C7-4A13-BD7B-ABD2BA248E56}">
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -1582,7 +1579,7 @@
     <col min="11" max="11" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="24" style="1" bestFit="1" customWidth="1"/>
@@ -1609,127 +1606,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:37" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:37" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AH2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AI2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1740,7 +1737,7 @@
       <c r="B3" s="1">
         <v>2023001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1234010112345</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1749,13 +1746,13 @@
       <c r="E3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -1773,7 +1770,7 @@
       <c r="M3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>39217</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -1809,7 +1806,7 @@
       <c r="Z3" s="1">
         <v>22345678</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="AB3" s="1" t="s">
@@ -1836,7 +1833,7 @@
       <c r="AJ3" s="1">
         <v>22345678</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AK3" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1847,7 +1844,7 @@
       <c r="B4" s="1">
         <v>2023002</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1234010112346</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1877,7 +1874,7 @@
       <c r="M4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>38696</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -1913,7 +1910,7 @@
       <c r="Y4" s="1">
         <v>9234567890</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AA4" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AB4" s="1" t="s">
@@ -1937,7 +1934,7 @@
       <c r="AI4" s="1">
         <v>8765432109</v>
       </c>
-      <c r="AK4" s="6" t="s">
+      <c r="AK4" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1945,7 +1942,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1234010112347</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1954,13 +1951,13 @@
       <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1972,7 +1969,7 @@
       <c r="M5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>41876</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -2023,7 +2020,7 @@
       <c r="AI5" s="1">
         <v>7654321098</v>
       </c>
-      <c r="AK5" s="6" t="s">
+      <c r="AK5" s="5" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2034,7 +2031,7 @@
       <c r="B6" s="1">
         <v>2023004</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1234010112349</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2061,7 +2058,7 @@
       <c r="M6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>35507</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -2094,7 +2091,7 @@
       <c r="Y6" s="1">
         <v>9456789012</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AA6" s="5" t="s">
         <v>103</v>
       </c>
       <c r="AB6" s="1" t="s">
@@ -2121,7 +2118,7 @@
       <c r="AJ6" s="1">
         <v>55555666</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AK6" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2129,7 +2126,7 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1234010112348</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2159,7 +2156,7 @@
       <c r="M7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>37777</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -2195,7 +2192,7 @@
       <c r="Z7" s="1">
         <v>66666777</v>
       </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AA7" s="5" t="s">
         <v>115</v>
       </c>
       <c r="AB7" s="1" t="s">
@@ -2222,7 +2219,7 @@
       <c r="AJ7" s="1">
         <v>9182301</v>
       </c>
-      <c r="AK7" s="6" t="s">
+      <c r="AK7" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2267,7 +2264,7 @@
     <col min="6" max="6" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="24" style="1" bestFit="1" customWidth="1"/>
@@ -2294,115 +2291,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:32" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:32" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2413,7 +2410,7 @@
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2431,7 +2428,7 @@
       <c r="H3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>39217</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -2467,7 +2464,7 @@
       <c r="U3" s="1">
         <v>22345678</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="W3" s="1" t="s">
@@ -2494,7 +2491,7 @@
       <c r="AE3" s="1">
         <v>22345678</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AF3" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2520,7 +2517,7 @@
       <c r="H4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>38696</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -2556,7 +2553,7 @@
       <c r="T4" s="1">
         <v>9234567890</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="V4" s="6" t="s">
         <v>78</v>
       </c>
       <c r="W4" s="1" t="s">
@@ -2580,7 +2577,7 @@
       <c r="AD4" s="1">
         <v>8765432109</v>
       </c>
-      <c r="AF4" s="6" t="s">
+      <c r="AF4" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2603,7 +2600,7 @@
       <c r="H5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>35507</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -2636,7 +2633,7 @@
       <c r="T5" s="1">
         <v>9456789012</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="5" t="s">
         <v>103</v>
       </c>
       <c r="W5" s="1" t="s">
@@ -2663,17 +2660,17 @@
       <c r="AE5" s="1">
         <v>55555666</v>
       </c>
-      <c r="AF5" s="6" t="s">
+      <c r="AF5" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2715,32 +2712,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2748,19 +2745,19 @@
       <c r="A3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2768,19 +2765,19 @@
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2788,19 +2785,19 @@
       <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2808,19 +2805,19 @@
       <c r="A6" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2828,19 +2825,19 @@
       <c r="A7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2848,19 +2845,19 @@
       <c r="A8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2868,19 +2865,19 @@
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2888,19 +2885,19 @@
       <c r="A10" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2908,19 +2905,19 @@
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2928,19 +2925,19 @@
       <c r="A12" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2948,19 +2945,19 @@
       <c r="A13" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2968,13 +2965,13 @@
       <c r="A14" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2988,10 +2985,10 @@
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" s="1">
@@ -3000,7 +2997,7 @@
       <c r="E15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3008,19 +3005,19 @@
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3028,19 +3025,19 @@
       <c r="A17" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="1">
         <v>4</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3048,19 +3045,19 @@
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="1">
         <v>3</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3068,19 +3065,19 @@
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3088,19 +3085,19 @@
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="E20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3111,16 +3108,16 @@
       <c r="B21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="D21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3131,16 +3128,16 @@
       <c r="B22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3151,16 +3148,16 @@
       <c r="B23" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="4" t="s">
+      <c r="E23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3171,16 +3168,16 @@
       <c r="B24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="4" t="s">
+      <c r="E24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3188,19 +3185,19 @@
       <c r="A25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="1">
         <v>3</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3208,10 +3205,10 @@
       <c r="A26" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1">
@@ -3220,7 +3217,7 @@
       <c r="E26" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3228,10 +3225,10 @@
       <c r="A27" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" s="1">
@@ -3240,7 +3237,7 @@
       <c r="E27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3248,10 +3245,10 @@
       <c r="A28" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="1">
@@ -3260,7 +3257,7 @@
       <c r="E28" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3268,19 +3265,19 @@
       <c r="A29" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="1">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="D29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3288,19 +3285,19 @@
       <c r="A30" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="1">
         <v>3</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3308,10 +3305,10 @@
       <c r="A31" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1">
@@ -3320,7 +3317,7 @@
       <c r="E31" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3340,8 +3337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE0AC57-319A-4A28-A178-4EB0E3F5AFD9}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3357,27 +3354,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3385,13 +3382,13 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>2023004</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3399,13 +3396,13 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>2023004</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3413,13 +3410,13 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>2023004</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3427,13 +3424,13 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>2023004</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3441,13 +3438,13 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>2023004</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3455,13 +3452,13 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>2023004</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3469,13 +3466,13 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>2023004</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3483,13 +3480,13 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>2023004</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3497,13 +3494,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>2023004</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3511,13 +3508,13 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>2023004</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3525,13 +3522,13 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>2023004</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3539,13 +3536,13 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>2023004</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3553,13 +3550,13 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <v>2023004</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3567,13 +3564,13 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>2023013</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3581,13 +3578,13 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>2023013</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3595,13 +3592,13 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>2023013</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3609,13 +3606,13 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>2023013</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3623,13 +3620,13 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>2023013</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3637,13 +3634,13 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>2023013</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3651,13 +3648,13 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>2023013</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3665,13 +3662,13 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="11">
         <v>2023013</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3679,13 +3676,13 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="11">
         <v>2023013</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3693,13 +3690,13 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="11">
         <v>2023013</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3707,13 +3704,13 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="11">
         <v>2023013</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3721,13 +3718,13 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>2023013</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3735,13 +3732,13 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="12">
         <v>2023023</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3749,13 +3746,13 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="12">
         <v>2023023</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3763,13 +3760,13 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <v>2023023</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3777,13 +3774,13 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <v>2023023</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3791,13 +3788,13 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="12">
         <v>2023023</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3805,13 +3802,13 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="12">
         <v>2023023</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3819,13 +3816,13 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="12">
         <v>2023023</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3833,13 +3830,13 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <v>2023023</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3847,13 +3844,13 @@
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <v>2023023</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3861,13 +3858,13 @@
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="12">
         <v>2023023</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="12" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3875,13 +3872,13 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="12">
         <v>2023023</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3889,13 +3886,13 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="12">
         <v>2023023</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3903,13 +3900,13 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="12">
         <v>2023023</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3917,13 +3914,13 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>2023023</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3931,13 +3928,13 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>2023023</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="12" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Sample DB Data xlsx
</commit_message>
<xml_diff>
--- a/docs/Sample DB Data.xlsx
+++ b/docs/Sample DB Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\TIP\ITE 001\FINAL PROJ\EnrollMe\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B507BC64-B56D-43B7-96FB-4109593190D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAF5DFC-0020-4AB6-A687-4D4C986EBEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{456103EC-7965-48E1-865D-F284B988141A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{456103EC-7965-48E1-865D-F284B988141A}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_enrollees" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="207">
   <si>
     <t>tbl_enrollees</t>
   </si>
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91B594-80C7-4A13-BD7B-ABD2BA248E56}">
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1980,6 +1980,9 @@
       <c r="K4" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="M4" s="1" t="s">
         <v>67</v>
       </c>
@@ -2072,8 +2075,14 @@
       <c r="I5" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="J5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>67</v>
@@ -2161,8 +2170,14 @@
       <c r="I6" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="J6" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>98</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>67</v>
@@ -2255,6 +2270,9 @@
       </c>
       <c r="I7" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>108</v>
@@ -2349,8 +2367,9 @@
     <hyperlink ref="AK7" r:id="rId9" xr:uid="{A74EC0E3-39F5-438C-8B3B-030E89B1CBE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2360,7 +2379,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G10" sqref="G10:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2759,8 +2778,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2769,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3777FB-1AB8-4F6A-A752-80A21C4B228A}">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3204,8 +3224,9 @@
     <hyperlink ref="AF5" r:id="rId6" xr:uid="{BCF94CB5-0E5A-4186-B4E5-AA674CCD146A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3215,7 +3236,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4051,8 +4072,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4061,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE0AC57-319A-4A28-A178-4EB0E3F5AFD9}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4668,8 +4690,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>